<commit_message>
Örnek girdi ve çıktı dosyaları düzenlendi.
</commit_message>
<xml_diff>
--- a/fiyat-dedektifi/urunler_sonuc.xlsx
+++ b/fiyat-dedektifi/urunler_sonuc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ceporjin-eticaret-fiyat-yonetimi\fiyat-dedektifi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15834E7E-49B4-4A0D-8479-35FC0B9F3415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71812D33-6964-4A28-BAC7-A2C037D0720B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,20 +46,20 @@
     <t>Samsung J7 Prime Batarya</t>
   </si>
   <si>
-    <t>KOD0001</t>
-  </si>
-  <si>
-    <t>KOD0002</t>
-  </si>
-  <si>
-    <t>KOD0003</t>
+    <t>KOD00001</t>
+  </si>
+  <si>
+    <t>KOD00002</t>
+  </si>
+  <si>
+    <t>KOD00003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +71,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -418,10 +424,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -492,6 +501,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>